<commit_message>
modifications on card statistics and help items
</commit_message>
<xml_diff>
--- a/Cards statistics.xlsx
+++ b/Cards statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -57,9 +57,6 @@
     <t xml:space="preserve">false </t>
   </si>
   <si>
-    <t xml:space="preserve">Advance to Electric Company utility square. If it is unowned If unowned, you may buy it from the Bank. If owned, then pay the rent accordingly. </t>
-  </si>
-  <si>
     <t>getEach</t>
   </si>
   <si>
@@ -70,16 +67,109 @@
   </si>
   <si>
     <t xml:space="preserve">It's you birthday. Collect 10$ from each player. </t>
+  </si>
+  <si>
+    <t>Bank error in your favor. Collect $200</t>
+  </si>
+  <si>
+    <t>Advance to Go. Collect $200</t>
+  </si>
+  <si>
+    <t>From sale of stock you get $50</t>
+  </si>
+  <si>
+    <t>Receive $25 consultancy fee</t>
+  </si>
+  <si>
+    <t>You inherit $100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advance to Electric Company utility square. If unowned, you may buy it from the Bank. If owned, then pay the rent accordingly. </t>
+  </si>
+  <si>
+    <t>Bank pays you dividend of $50</t>
+  </si>
+  <si>
+    <t>Go Back 3 Spaces</t>
+  </si>
+  <si>
+    <t>Pay poor tax of $15</t>
+  </si>
+  <si>
+    <t>Doctor's fees. Pay $50</t>
+  </si>
+  <si>
+    <t>Grand Opera Night. Collect $50 from every player for opening night seats</t>
+  </si>
+  <si>
+    <t>Holiday Fund matures. Receive $100</t>
+  </si>
+  <si>
+    <t>Income tax refund. Collect $20</t>
+  </si>
+  <si>
+    <t>Life insurance matures. Collect $100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pay hospital fees of $100 </t>
+  </si>
+  <si>
+    <t>Pay school fees of $150</t>
+  </si>
+  <si>
+    <t>You have won second prize in a beauty contest. Collect $10</t>
+  </si>
+  <si>
+    <t>Go to Jail directly. Do not pass Go, do not collect $200</t>
+  </si>
+  <si>
+    <t>Make general repairs on all your property.For each house pay $25, for each hotel $100</t>
+  </si>
+  <si>
+    <t>Take a trip to Reading Railroad. If you pass Go, collect $200</t>
+  </si>
+  <si>
+    <t>Your building {and} loan matures. Collect $150</t>
+  </si>
+  <si>
+    <t>You have won a crossword competition. Collect $100</t>
+  </si>
+  <si>
+    <t>Get out of Jail Free. This card may be kept until needed, or traded/sold </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
@@ -103,13 +193,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -462,7 +558,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2">
@@ -488,7 +584,7 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F3">
@@ -514,7 +610,7 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F4">
@@ -540,81 +636,274 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
+      </c>
+      <c r="B10">
+        <v>-15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>150</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>13</v>
-      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>15</v>
-      </c>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E7" r:id="rId1" tooltip="Go Back 3 Spaces" display="http://monopoly.wikia.com/wiki/Go_Back_3_Spaces"/>
+    <hyperlink ref="E14" r:id="rId2" tooltip="Get out of Jail Free (card)" display="http://monopoly.wikia.com/wiki/Get_out_of_Jail_Free_(card)"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,11 +931,26 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
@@ -654,16 +958,61 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>-50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -676,10 +1025,10 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -689,20 +1038,80 @@
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -718,8 +1127,8 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
-        <v>17</v>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -729,34 +1138,131 @@
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>-100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>-150</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E18" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E7" r:id="rId1" tooltip="Jail" display="http://monopoly.wikia.com/wiki/Jail"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>